<commit_message>
fix & added current_user
</commit_message>
<xml_diff>
--- a/expense.xlsx
+++ b/expense.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>Borrower Name</t>
+  </si>
+  <si>
+    <t>2022-01-13 16:50:17.078917</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>qcvcvbcvy</t>
+  </si>
+  <si>
+    <t>2022-01-13 16:50:26.841231</t>
   </si>
 </sst>
 </file>
@@ -74,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,6 +112,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some errors 3
</commit_message>
<xml_diff>
--- a/expense.xlsx
+++ b/expense.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>Borrower Name</t>
+  </si>
+  <si>
+    <t>2022-01-13 16:50:17.078917</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>qcvcvbcvy</t>
+  </si>
+  <si>
+    <t>2022-01-13 16:50:26.841231</t>
   </si>
 </sst>
 </file>
@@ -74,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,6 +112,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
renamed security dir & updated design
</commit_message>
<xml_diff>
--- a/expense.xlsx
+++ b/expense.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>#</t>
   </si>
@@ -32,16 +32,28 @@
     <t>Borrower Name</t>
   </si>
   <si>
-    <t>2022-01-13 16:50:17.078917</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>qcvcvbcvy</t>
-  </si>
-  <si>
-    <t>2022-01-13 16:50:26.841231</t>
+    <t>2022-01-19 20:07:54.443948</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>2022-01-19 21:51:18.819872</t>
+  </si>
+  <si>
+    <t>UAH</t>
+  </si>
+  <si>
+    <t>2022-01-19 21:51:44.560407</t>
+  </si>
+  <si>
+    <t>2022-01-19 21:52:56.170675</t>
   </si>
 </sst>
 </file>
@@ -86,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,13 +126,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>500.0</v>
+        <v>10000.0</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -129,26 +141,66 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>500.0</v>
+        <v>5.8895544E7</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2375821.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>